<commit_message>
summarize findings for facebook
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C230024-7EAD-4EF1-BACB-0A4B44F3F1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBBDCD4-E583-48A1-B0DF-965C6A9C74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Count</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>(Tolerance) partial functionality</t>
+  </si>
+  <si>
+    <t>Concurrency</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>(Concurrency) locks</t>
+  </si>
+  <si>
+    <t>Async Wait</t>
+  </si>
+  <si>
+    <t>(Async Wait) added waitFor</t>
+  </si>
+  <si>
+    <t>(Memory) added memory for test</t>
   </si>
 </sst>
 </file>
@@ -441,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F24"/>
+  <dimension ref="B3:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -526,6 +544,12 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
@@ -534,6 +558,12 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
@@ -557,6 +587,30 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>4</v>
@@ -594,7 +648,7 @@
         <v>12</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
@@ -611,6 +665,14 @@
       </c>
       <c r="C24">
         <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summarize findings for microsoft, stripe
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBBDCD4-E583-48A1-B0DF-965C6A9C74AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2E7F80-887D-4196-AF13-E36FEEBEE377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Count</t>
   </si>
@@ -57,12 +57,6 @@
     <t>TypeScript</t>
   </si>
   <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Dependencies) update </t>
-  </si>
-  <si>
     <t>Python</t>
   </si>
   <si>
@@ -109,6 +103,27 @@
   </si>
   <si>
     <t>(Memory) added memory for test</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>(Delay) add custom delay / wait</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Kotlin</t>
+  </si>
+  <si>
+    <t>Dependencies / Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Dependencies / Environment) update </t>
   </si>
 </sst>
 </file>
@@ -459,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F25"/>
+  <dimension ref="B3:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,13 +507,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -517,27 +532,27 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -545,35 +560,41 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>20</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -581,7 +602,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -589,7 +610,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -597,18 +618,26 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
@@ -632,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
@@ -645,7 +674,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -653,7 +682,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -661,7 +690,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>9</v>
@@ -669,10 +698,34 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summarize findings for twosigma, uber
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2E7F80-887D-4196-AF13-E36FEEBEE377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC6F41-77FA-4C78-9A81-A7E39601948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Count</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t xml:space="preserve">(Dependencies / Environment) update </t>
+  </si>
+  <si>
+    <t>Clojure</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>(Collections) sort / establish ordering</t>
+  </si>
+  <si>
+    <t>(Collections) limit elements</t>
   </si>
 </sst>
 </file>
@@ -190,8 +202,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F16" totalsRowShown="0">
-  <autoFilter ref="E3:F16" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F17" totalsRowShown="0">
+  <autoFilter ref="E3:F17" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5D3E98C6-B9C7-4DB9-B67A-0ED3228E11E1}" name="RQ2: Fix for Flakiness?"/>
     <tableColumn id="2" xr3:uid="{829AB046-7D25-4B45-ADCD-65F6668ED8A6}" name="Count"/>
@@ -474,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F28"/>
+  <dimension ref="B3:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,13 +519,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -563,7 +575,7 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -601,6 +613,12 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
@@ -613,7 +631,7 @@
         <v>22</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
@@ -640,7 +658,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>4</v>
       </c>
@@ -648,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -656,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -664,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -672,15 +706,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -688,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -696,7 +730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -704,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>26</v>
       </c>
@@ -712,20 +746,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>30</v>
       </c>
       <c r="C28">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summarize findings for google
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC6F41-77FA-4C78-9A81-A7E39601948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15752ED-0E68-4B97-AD84-6D4253B6EBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Count</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>(Collections) limit elements</t>
+  </si>
+  <si>
+    <t>Bit Manipulation / Arithmetic</t>
+  </si>
+  <si>
+    <t>(Bit Manipulation / Arithmetic) bit clear</t>
+  </si>
+  <si>
+    <t>(Concurrency) update global state</t>
+  </si>
+  <si>
+    <t>Rust</t>
+  </si>
+  <si>
+    <t>(Async Wait) Promise statement</t>
   </si>
 </sst>
 </file>
@@ -202,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F17" totalsRowShown="0">
-  <autoFilter ref="E3:F17" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F20" totalsRowShown="0">
+  <autoFilter ref="E3:F20" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5D3E98C6-B9C7-4DB9-B67A-0ED3228E11E1}" name="RQ2: Fix for Flakiness?"/>
     <tableColumn id="2" xr3:uid="{829AB046-7D25-4B45-ADCD-65F6668ED8A6}" name="Count"/>
@@ -213,8 +228,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}" name="Table3" displayName="Table3" ref="B18:C29" totalsRowShown="0">
-  <autoFilter ref="B18:C29" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}" name="Table3" displayName="Table3" ref="B18:C30" totalsRowShown="0">
+  <autoFilter ref="B18:C30" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F0068822-083B-4BDB-99B5-6ACC44D4E438}" name="Programming Language"/>
     <tableColumn id="2" xr3:uid="{840AB94B-1139-41EF-B336-F06393B2838D}" name="Count"/>
@@ -486,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F29"/>
+  <dimension ref="B3:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,13 +534,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -533,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
@@ -547,13 +562,13 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
@@ -561,13 +576,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
@@ -575,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -589,13 +604,13 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
@@ -603,7 +618,7 @@
         <v>27</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -617,7 +632,7 @@
         <v>34</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
@@ -627,6 +642,12 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
@@ -639,7 +660,7 @@
         <v>24</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.35">
@@ -655,7 +676,7 @@
         <v>28</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
@@ -663,7 +684,7 @@
         <v>35</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
@@ -681,6 +702,12 @@
       <c r="C18" t="s">
         <v>0</v>
       </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
@@ -689,6 +716,12 @@
       <c r="C19">
         <v>1</v>
       </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
@@ -697,13 +730,19 @@
       <c r="C20">
         <v>10</v>
       </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
@@ -711,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
@@ -719,7 +758,7 @@
         <v>15</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
@@ -735,7 +774,7 @@
         <v>21</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
@@ -751,7 +790,7 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
@@ -759,7 +798,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
@@ -768,6 +807,14 @@
       </c>
       <c r="C29">
         <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates based on progress report 2 feedback
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E14487-A37D-4A3E-9099-B7A3525FE8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5582AF35-DD65-46FB-BAF7-C4D64A5328A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,9 +47,6 @@
     <t>RQ2: Fix for Flakiness?</t>
   </si>
   <si>
-    <t>Tolerance</t>
-  </si>
-  <si>
     <t>Programming Language</t>
   </si>
   <si>
@@ -51,9 +59,6 @@
     <t>Memory</t>
   </si>
   <si>
-    <t>(Memory) deallocate unused space</t>
-  </si>
-  <si>
     <t>TypeScript</t>
   </si>
   <si>
@@ -63,54 +68,27 @@
     <t>Order of Events</t>
   </si>
   <si>
-    <t>(Order of Events) implement event ordering</t>
-  </si>
-  <si>
-    <t>(Tolerance) update conditionals</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
-    <t>(Order of Events) setup state</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
-    <t>(Order of Events) tear down state after shutdown</t>
-  </si>
-  <si>
-    <t>(Tolerance) partial functionality</t>
-  </si>
-  <si>
     <t>Concurrency</t>
   </si>
   <si>
     <t>C++</t>
   </si>
   <si>
-    <t>(Concurrency) locks</t>
-  </si>
-  <si>
     <t>Async Wait</t>
   </si>
   <si>
-    <t>(Async Wait) added waitFor</t>
-  </si>
-  <si>
-    <t>(Memory) added memory for test</t>
-  </si>
-  <si>
     <t>C#</t>
   </si>
   <si>
     <t>Delay</t>
   </si>
   <si>
-    <t>(Delay) add custom delay / wait</t>
-  </si>
-  <si>
     <t>Go</t>
   </si>
   <si>
@@ -120,49 +98,82 @@
     <t>Dependencies / Environment</t>
   </si>
   <si>
-    <t xml:space="preserve">(Dependencies / Environment) update </t>
-  </si>
-  <si>
     <t>Clojure</t>
   </si>
   <si>
     <t>Collections</t>
   </si>
   <si>
-    <t>(Collections) sort / establish ordering</t>
-  </si>
-  <si>
-    <t>(Collections) limit elements</t>
-  </si>
-  <si>
     <t>Bit Manipulation / Arithmetic</t>
   </si>
   <si>
-    <t>(Bit Manipulation / Arithmetic) bit clear</t>
-  </si>
-  <si>
-    <t>(Concurrency) update global state</t>
-  </si>
-  <si>
     <t>Rust</t>
   </si>
   <si>
-    <t>(Async Wait) Promise statement</t>
-  </si>
-  <si>
-    <t>(Dependencies / Environment) remove dependencies</t>
-  </si>
-  <si>
     <t>Comparisons</t>
   </si>
   <si>
-    <t>(Comparisons) same type</t>
-  </si>
-  <si>
-    <t>(Bit Manipulation / Arithmetic) no hardcoded values</t>
-  </si>
-  <si>
-    <t>(Tolerance) relax acceptance/tolerance</t>
+    <t>Algorithmic Flakiness</t>
+  </si>
+  <si>
+    <t>Incorrect Logic</t>
+  </si>
+  <si>
+    <t>relax acceptance/tolerance</t>
+  </si>
+  <si>
+    <t>deallocate unused space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update </t>
+  </si>
+  <si>
+    <t>implement event ordering</t>
+  </si>
+  <si>
+    <t>refactor program logic</t>
+  </si>
+  <si>
+    <t>setup state</t>
+  </si>
+  <si>
+    <t>tear down state after shutdown</t>
+  </si>
+  <si>
+    <t>no hardcoded values</t>
+  </si>
+  <si>
+    <t>same type</t>
+  </si>
+  <si>
+    <t>remove dependencies</t>
+  </si>
+  <si>
+    <t>Promise statement</t>
+  </si>
+  <si>
+    <t>update global state</t>
+  </si>
+  <si>
+    <t>bit clear</t>
+  </si>
+  <si>
+    <t>limit elements</t>
+  </si>
+  <si>
+    <t>sort / establish ordering</t>
+  </si>
+  <si>
+    <t>add custom delay / wait</t>
+  </si>
+  <si>
+    <t>added memory for test</t>
+  </si>
+  <si>
+    <t>added waitFor</t>
+  </si>
+  <si>
+    <t>locks</t>
   </si>
 </sst>
 </file>
@@ -218,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B2608637-C130-4393-ABCD-A6A790E1F84A}" name="Table1" displayName="Table1" ref="B3:C16" totalsRowShown="0">
-  <autoFilter ref="B3:C16" xr:uid="{B2608637-C130-4393-ABCD-A6A790E1F84A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B2608637-C130-4393-ABCD-A6A790E1F84A}" name="Table1" displayName="Table1" ref="B3:C15" totalsRowShown="0">
+  <autoFilter ref="B3:C15" xr:uid="{B2608637-C130-4393-ABCD-A6A790E1F84A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{587C579E-36BB-4E18-8383-3274037924AE}" name="RQ1: Cause of Flakiness?"/>
     <tableColumn id="2" xr3:uid="{610F1FAF-8A7C-411F-A63E-63F53C704DC1}" name="Count"/>
@@ -229,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F23" totalsRowShown="0">
-  <autoFilter ref="E3:F23" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}" name="Table13" displayName="Table13" ref="E3:F23" totalsRowCount="1">
+  <autoFilter ref="E3:F22" xr:uid="{4AF1DB72-6A4C-4B94-B13D-D91A4515B672}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5D3E98C6-B9C7-4DB9-B67A-0ED3228E11E1}" name="RQ2: Fix for Flakiness?"/>
     <tableColumn id="2" xr3:uid="{829AB046-7D25-4B45-ADCD-65F6668ED8A6}" name="Count"/>
@@ -240,8 +251,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}" name="Table3" displayName="Table3" ref="B18:C30" totalsRowShown="0">
-  <autoFilter ref="B18:C30" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}" name="Table3" displayName="Table3" ref="B17:C29" totalsRowShown="0">
+  <autoFilter ref="B17:C29" xr:uid="{5DC2FD8C-971C-4E9C-B125-F25DCFBD1121}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F0068822-083B-4BDB-99B5-6ACC44D4E438}" name="Programming Language"/>
     <tableColumn id="2" xr3:uid="{840AB94B-1139-41EF-B336-F06393B2838D}" name="Count"/>
@@ -513,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F30"/>
+  <dimension ref="B3:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,27 +554,27 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F4">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -571,13 +582,13 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -585,13 +596,13 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -599,27 +610,27 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8">
         <v>13</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -627,13 +638,13 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F10">
         <v>11</v>
@@ -641,73 +652,85 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
       <c r="F14">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -717,11 +740,11 @@
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
-        <v>0</v>
+      <c r="C18">
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -732,10 +755,10 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -743,30 +766,30 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20">
         <v>6</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
@@ -774,82 +797,68 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-calculate RQ1 up through google
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA6102-A51F-477F-945E-A0A7152B94AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F7025-A681-4693-9BD8-79E9DDBA59EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Count</t>
   </si>
@@ -183,6 +183,30 @@
   </si>
   <si>
     <t>skip tests</t>
+  </si>
+  <si>
+    <t>incorrect program logic</t>
+  </si>
+  <si>
+    <t>algorithmic flakiness</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>async wait</t>
+  </si>
+  <si>
+    <t>unordered collections</t>
+  </si>
+  <si>
+    <t>concurrency</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>arithmetic/bit operations</t>
   </si>
 </sst>
 </file>
@@ -533,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F30"/>
+  <dimension ref="B3:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +571,7 @@
     <col min="6" max="6" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -561,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -574,8 +598,14 @@
       <c r="F4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -588,8 +618,14 @@
       <c r="F5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -602,8 +638,14 @@
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -616,8 +658,14 @@
       <c r="F7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -630,8 +678,14 @@
       <c r="F8">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -644,8 +698,14 @@
       <c r="F9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -658,8 +718,14 @@
       <c r="F10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -672,8 +738,14 @@
       <c r="F11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -687,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -701,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -715,7 +787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
         <v>40</v>
       </c>
@@ -723,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
finish updates for RQ1 findings
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knkes\Documents\UT Austin\Semesters\Fall 2022\ECE 382V\ECE382V_An_Empirical_Analysis_of_Flaky_Tests_In_Industry_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F7025-A681-4693-9BD8-79E9DDBA59EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC99348-F92A-4801-9211-B454B943072C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Count</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>Order of Events</t>
-  </si>
-  <si>
     <t>JavaScript</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>C#</t>
   </si>
   <si>
-    <t>Delay</t>
-  </si>
-  <si>
     <t>Go</t>
   </si>
   <si>
@@ -110,15 +104,9 @@
     <t>Rust</t>
   </si>
   <si>
-    <t>Comparisons</t>
-  </si>
-  <si>
     <t>Algorithmic Flakiness</t>
   </si>
   <si>
-    <t>Incorrect Logic</t>
-  </si>
-  <si>
     <t>relax acceptance/tolerance</t>
   </si>
   <si>
@@ -185,28 +173,7 @@
     <t>skip tests</t>
   </si>
   <si>
-    <t>incorrect program logic</t>
-  </si>
-  <si>
-    <t>algorithmic flakiness</t>
-  </si>
-  <si>
-    <t>environment</t>
-  </si>
-  <si>
-    <t>async wait</t>
-  </si>
-  <si>
-    <t>unordered collections</t>
-  </si>
-  <si>
-    <t>concurrency</t>
-  </si>
-  <si>
-    <t>memory</t>
-  </si>
-  <si>
-    <t>arithmetic/bit operations</t>
+    <t>Incorrect Program Logic</t>
   </si>
 </sst>
 </file>
@@ -557,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K30"/>
+  <dimension ref="B3:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +538,7 @@
     <col min="6" max="6" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -585,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -593,211 +560,145 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>8</v>
       </c>
-      <c r="H7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <v>31</v>
       </c>
-      <c r="H8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>11</v>
       </c>
-      <c r="H10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
-      <c r="H11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>14</v>
-      </c>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -811,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -825,7 +726,7 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -839,7 +740,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -853,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -867,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -875,13 +776,13 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -889,13 +790,13 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -903,13 +804,13 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -917,7 +818,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -925,7 +826,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -933,7 +834,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27">
         <v>9</v>
@@ -941,7 +842,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -949,7 +850,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -957,7 +858,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C30">
         <v>2</v>

</xml_diff>